<commit_message>
Added Comments for Method in Home Page
</commit_message>
<xml_diff>
--- a/src/test/resources/testResources/DataDrivenTestingTest.xlsx
+++ b/src/test/resources/testResources/DataDrivenTestingTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1331,7 +1331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
@@ -3152,7 +3152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>